<commit_message>
21st Dec 2024 Test Script Design
</commit_message>
<xml_diff>
--- a/TestData/10thAug24.xlsx
+++ b/TestData/10thAug24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\10th Aug 2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\10th Aug 2024\Workspace\10ThAug24_Framework_MavenProject\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2A0C1A-E70E-475D-958F-A9D65098E121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFBB2E3-BF9C-487A-9FBA-1CB249CEE897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
   <si>
     <t>Asci/Hash Value</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Swag Labs</t>
   </si>
   <si>
-    <t>Password is required</t>
-  </si>
-  <si>
     <t>sr no</t>
   </si>
   <si>
@@ -150,13 +147,16 @@
   </si>
   <si>
     <t>enter bug ID</t>
+  </si>
+  <si>
+    <t>Sauce Labs Onesie</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +179,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF171D1E"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -217,12 +224,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -757,15 +765,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5E6CFC-672F-490F-A3F6-138BD02FA2CF}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
   </cols>
@@ -782,11 +790,23 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
+      <c r="A2" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>7.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>129.94</v>
       </c>
     </row>
   </sheetData>
@@ -798,7 +818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6FDE49A-B30D-4E6B-9FDD-B2F37FAE7016}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
@@ -812,34 +832,34 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -847,10 +867,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -858,10 +878,10 @@
         <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -871,23 +891,23 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E3" s="1"/>
       <c r="I3" s="1">
         <v>2</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -897,10 +917,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -908,10 +928,10 @@
         <v>3</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -921,10 +941,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -932,10 +952,10 @@
         <v>4</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -945,29 +965,29 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="1"/>
       <c r="I6" s="1">
         <v>5</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
@@ -975,10 +995,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -986,20 +1006,20 @@
         <v>6</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" t="s">
         <v>35</v>
-      </c>
-      <c r="K11" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
23rd dec Test Script Design
</commit_message>
<xml_diff>
--- a/TestData/10thAug24.xlsx
+++ b/TestData/10thAug24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\10th Aug 2024\Workspace\10ThAug24_Framework_MavenProject\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFBB2E3-BF9C-487A-9FBA-1CB249CEE897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63CBE65-0E0F-4079-8469-DC26DEC5A5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="42">
   <si>
     <t>Asci/Hash Value</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>Sauce Labs Onesie</t>
+  </si>
+  <si>
+    <t>Your order has been dispatched, and will arrive just as fast as the pony can get there!</t>
+  </si>
+  <si>
+    <t>111</t>
   </si>
 </sst>
 </file>
@@ -765,10 +771,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5E6CFC-672F-490F-A3F6-138BD02FA2CF}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -776,9 +782,10 @@
     <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -789,24 +796,38 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>7.99</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>129.94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>